<commit_message>
feat: add database schema and data dummy data report
</commit_message>
<xml_diff>
--- a/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
+++ b/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/zulfano_pramono_binus_ac_id/Documents/Skripsi/Whatsapp Bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/zulfano_pramono_binus_ac_id/Documents/Skripsi/implementasi_whatsapp_bot/dokumentasi/perencanaan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3961AB6-C70B-4613-8247-9842956BE957}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DC2718-A402-4BD3-A357-DF6B65046064}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{124ADDE1-F12C-4139-A46F-F89A61D9CD17}"/>
   </bookViews>
@@ -801,7 +801,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -897,7 +897,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -918,7 +918,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -939,7 +939,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -960,7 +960,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -981,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="F8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -1002,7 +1002,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2"/>
     </row>

</xml_diff>

<commit_message>
feat: implement basic whatsapp bot ping pong
</commit_message>
<xml_diff>
--- a/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
+++ b/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/zulfano_pramono_binus_ac_id/Documents/Skripsi/implementasi_whatsapp_bot/dokumentasi/perencanaan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DC2718-A402-4BD3-A357-DF6B65046064}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D61DC9-B740-4047-88FC-7B142A7E92C3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{124ADDE1-F12C-4139-A46F-F89A61D9CD17}"/>
   </bookViews>
@@ -801,7 +801,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1023,7 +1023,7 @@
         <v>37</v>
       </c>
       <c r="F10" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -1044,7 +1044,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -1065,7 +1065,7 @@
         <v>43</v>
       </c>
       <c r="F12" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2"/>
     </row>

</xml_diff>

<commit_message>
feat: add mysql database connection
</commit_message>
<xml_diff>
--- a/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
+++ b/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/zulfano_pramono_binus_ac_id/Documents/Skripsi/implementasi_whatsapp_bot/dokumentasi/perencanaan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D61DC9-B740-4047-88FC-7B142A7E92C3}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21A59E1D-7B92-49CE-A90F-ABBF9B9FF739}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{124ADDE1-F12C-4139-A46F-F89A61D9CD17}"/>
   </bookViews>
@@ -390,12 +390,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -425,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -445,6 +451,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -800,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6B48D4-919A-4412-9EB5-5665C38E690E}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,19 +848,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3" t="b">
@@ -860,19 +869,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="3" t="b">
@@ -881,19 +890,19 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="3" t="b">
@@ -902,19 +911,19 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="3" t="b">
@@ -923,19 +932,19 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="3" t="b">
@@ -944,19 +953,19 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="3" t="b">
@@ -965,19 +974,19 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F8" s="3" t="b">
@@ -986,19 +995,19 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="3" t="b">
@@ -1007,19 +1016,19 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F10" s="3" t="b">
@@ -1028,19 +1037,19 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="3" t="b">
@@ -1049,19 +1058,19 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="3" t="b">
@@ -1070,86 +1079,86 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F16" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2"/>
     </row>

</xml_diff>

<commit_message>
feat: add whitelist-based logging for bot commands
</commit_message>
<xml_diff>
--- a/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
+++ b/dokumentasi/perencanaan/02_tracker_progres_skripsi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/zulfano_pramono_binus_ac_id/Documents/Skripsi/implementasi_whatsapp_bot/dokumentasi/perencanaan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zulfano\Zulfano\Binus\implementasi_whatsapp_bot\dokumentasi\perencanaan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{89827C79-9484-4663-BE16-259E17F9FE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21A59E1D-7B92-49CE-A90F-ABBF9B9FF739}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BB42A7-71C0-4C8A-B6A9-0C604A614D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{124ADDE1-F12C-4139-A46F-F89A61D9CD17}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="115">
   <si>
     <t>No</t>
   </si>
@@ -367,6 +367,24 @@
   </si>
   <si>
     <t>v2.x</t>
+  </si>
+  <si>
+    <t>API manajemen whitelist</t>
+  </si>
+  <si>
+    <t>CRUD whitelist</t>
+  </si>
+  <si>
+    <t>Endpoint API</t>
+  </si>
+  <si>
+    <t>UI React untuk manajemen whitelist</t>
+  </si>
+  <si>
+    <t>UI whitelist</t>
+  </si>
+  <si>
+    <t>Screenshot UI</t>
   </si>
 </sst>
 </file>
@@ -431,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -456,6 +474,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,15 +834,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6B48D4-919A-4412-9EB5-5665C38E690E}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
@@ -1163,146 +1190,146 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F18" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="A19" s="9">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
+        <v>17.2</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E21" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="F21" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F22" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F23" s="3" t="b">
         <v>0</v>
@@ -1311,19 +1338,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="F24" s="3" t="b">
         <v>0</v>
@@ -1332,19 +1359,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F25" s="3" t="b">
         <v>0</v>
@@ -1353,19 +1380,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="F26" s="3" t="b">
         <v>0</v>
@@ -1374,19 +1401,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F27" s="3" t="b">
         <v>0</v>
@@ -1395,19 +1422,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F28" s="3" t="b">
         <v>0</v>
@@ -1416,19 +1443,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F29" s="3" t="b">
         <v>0</v>
@@ -1437,27 +1464,69 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F30" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G30" s="2"/>
     </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>29</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G30" xr:uid="{7C6B48D4-919A-4412-9EB5-5665C38E690E}"/>
+  <autoFilter ref="A1:G32" xr:uid="{7C6B48D4-919A-4412-9EB5-5665C38E690E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>